<commit_message>
1. Select treenode after delete. 2. TreeNodes are sorted! If there's a problem with time, method can be changed.
</commit_message>
<xml_diff>
--- a/Утилита трудозатрат пожелания.xlsx
+++ b/Утилита трудозатрат пожелания.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\_УчётТрудозатрат\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\-staff-time\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="89">
   <si>
     <t>Дата</t>
   </si>
@@ -368,12 +368,21 @@
 2. Исходя из диапазона должно рассчитываться количество минут, сейчас такое впечатление, что время окончания считается как время начала + количество минут (т.к. не могу скорректировать время окончания, оно становится автоматом при указания количества минут);
 3. Рассчет времени странный ставлю время начала 9:15:00, длительность 45 минут, время окончания посчитал 10:19:11, хотя должно быть 10:00:00.</t>
   </si>
+  <si>
+    <t>Обсуждение</t>
+  </si>
+  <si>
+    <t>Добавить поле в бд. Если для каждого пользователя свое поле, то в таблицу связей пользователя с задачей.</t>
+  </si>
+  <si>
+    <t>Желательно еще потестить поведение</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -402,6 +411,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="204"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
@@ -447,8 +464,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -504,8 +520,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -595,23 +612,24 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="4" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Нейтральный" xfId="1" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -892,9 +910,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1125,23 +1143,23 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="12">
         <v>43248</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="31" t="s">
+      <c r="E10" s="13"/>
+      <c r="F10" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="29"/>
+      <c r="G10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
@@ -1235,23 +1253,23 @@
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="9">
         <v>43248</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="31" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="29"/>
+      <c r="G15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -1305,41 +1323,45 @@
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="9">
         <v>43256</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="29"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="32">
         <v>43256</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="33" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="33" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="29"/>
+      <c r="E19" s="34"/>
+      <c r="F19" s="34"/>
+      <c r="G19" s="34" t="s">
+        <v>86</v>
+      </c>
+      <c r="H19" s="34" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -1367,21 +1389,23 @@
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="9">
         <v>43256</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="29"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -1461,8 +1485,12 @@
         <v>68</v>
       </c>
       <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="F25" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1533,21 +1561,23 @@
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="9">
         <v>43257</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -1628,28 +1658,32 @@
       <c r="H33" s="34"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="35">
         <v>33</v>
       </c>
-      <c r="B34" s="28">
+      <c r="B34" s="9">
         <v>43257</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="35">
+      <c r="B35" s="31">
         <v>43271</v>
       </c>
       <c r="C35" s="6" t="s">
@@ -1657,13 +1691,16 @@
       </c>
       <c r="D35" s="7" t="s">
         <v>83</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="35">
+      <c r="B36" s="31">
         <v>43271</v>
       </c>
       <c r="C36" s="6" t="s">
@@ -1671,13 +1708,19 @@
       </c>
       <c r="D36" s="7" t="s">
         <v>84</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="35">
+      <c r="B37" s="31">
         <v>43271</v>
       </c>
       <c r="C37" s="6" t="s">
@@ -1685,6 +1728,15 @@
       </c>
       <c r="D37" s="7" t="s">
         <v>85</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>88</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Works are sorted, don't change their order after edit anymore.
</commit_message>
<xml_diff>
--- a/Утилита трудозатрат пожелания.xlsx
+++ b/Утилита трудозатрат пожелания.xlsx
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="89">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="88">
   <si>
     <t>Дата</t>
   </si>
@@ -343,9 +343,6 @@
     <t>Ввод времени работы: минуты + время начала. Можно обговорить другой вариант.</t>
   </si>
   <si>
-    <t>Дерево</t>
-  </si>
-  <si>
     <t>Невозможно вызвать два редактирования задачи</t>
   </si>
   <si>
@@ -382,7 +379,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -411,13 +408,6 @@
     </font>
     <font>
       <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <charset val="204"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
       <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -425,7 +415,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -453,12 +443,6 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFF0000"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -522,9 +506,9 @@
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -591,41 +575,26 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="4" fillId="7" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="7" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -911,8 +880,8 @@
   <dimension ref="A1:H1000"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A31" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G37" sqref="G37"/>
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -976,26 +945,26 @@
       <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="12">
         <v>43248</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1024,28 +993,24 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="29">
         <v>4</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="25">
         <v>43248</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="27" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="25" t="s">
+      <c r="E5" s="27"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="25" t="s">
-        <v>79</v>
-      </c>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1292,7 +1257,7 @@
         <v>36</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1309,14 +1274,12 @@
         <v>60</v>
       </c>
       <c r="E17" s="18"/>
-      <c r="F17" s="20" t="s">
-        <v>29</v>
-      </c>
+      <c r="F17" s="20"/>
       <c r="G17" s="18" t="s">
         <v>37</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1345,22 +1308,22 @@
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="32">
+      <c r="B19" s="25">
         <v>43256</v>
       </c>
-      <c r="C19" s="33" t="s">
+      <c r="C19" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="33" t="s">
+      <c r="D19" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34" t="s">
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="27" t="s">
         <v>86</v>
-      </c>
-      <c r="H19" s="34" t="s">
-        <v>87</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
@@ -1514,7 +1477,7 @@
         <v>36</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -1543,19 +1506,19 @@
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="32">
+      <c r="B28" s="25">
         <v>43256</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
@@ -1623,42 +1586,42 @@
       <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="25">
         <v>43257</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="32">
+      <c r="B33" s="25">
         <v>43257</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="35">
+      <c r="A34" s="28">
         <v>33</v>
       </c>
       <c r="B34" s="9">
@@ -1683,14 +1646,14 @@
       <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="31">
+      <c r="B35" s="24">
         <v>43271</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="F35" s="6" t="s">
         <v>29</v>
@@ -1700,14 +1663,14 @@
       <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="31">
+      <c r="B36" s="24">
         <v>43271</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="F36" s="6" t="s">
         <v>29</v>
@@ -1720,14 +1683,14 @@
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="31">
+      <c r="B37" s="24">
         <v>43271</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="F37" s="6" t="s">
         <v>29</v>
@@ -1736,7 +1699,7 @@
         <v>36</v>
       </c>
       <c r="H37" s="6" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Selection and Expanison are added, works and tasks are in order
</commit_message>
<xml_diff>
--- a/Утилита трудозатрат пожелания.xlsx
+++ b/Утилита трудозатрат пожелания.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="M:\_УчётТрудозатрат\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\-staff-time\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="177" uniqueCount="86">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="188" uniqueCount="88">
   <si>
     <t>Дата</t>
   </si>
@@ -343,9 +343,6 @@
     <t>Ввод времени работы: минуты + время начала. Можно обговорить другой вариант.</t>
   </si>
   <si>
-    <t>Дерево</t>
-  </si>
-  <si>
     <t>Невозможно вызвать два редактирования задачи</t>
   </si>
   <si>
@@ -368,11 +365,20 @@
 2. Исходя из диапазона должно рассчитываться количество минут, сейчас такое впечатление, что время окончания считается как время начала + количество минут (т.к. не могу скорректировать время окончания, оно становится автоматом при указания количества минут);
 3. Рассчет времени странный ставлю время начала 9:15:00, длительность 45 минут, время окончания посчитал 10:19:11, хотя должно быть 10:00:00.</t>
   </si>
+  <si>
+    <t>Обсуждение</t>
+  </si>
+  <si>
+    <t>Добавить поле в бд. Если для каждого пользователя свое поле, то в таблицу связей пользователя с задачей.</t>
+  </si>
+  <si>
+    <t>Желательно еще потестить поведение</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -402,13 +408,14 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF9C6500"/>
       <name val="Calibri"/>
       <family val="2"/>
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -441,14 +448,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FF00B050"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FF0070C0"/>
-        <bgColor indexed="64"/>
+        <fgColor rgb="FFFFEB9C"/>
       </patternFill>
     </fill>
   </fills>
@@ -504,10 +504,11 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -574,44 +575,30 @@
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="6" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="14" fontId="0" fillId="7" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="6" borderId="1" xfId="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Нейтральный" xfId="1" builtinId="28"/>
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -892,9 +879,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:H1000"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A32" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D38" sqref="D38"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A14" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D21" sqref="D21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -958,26 +945,26 @@
       <c r="H2" s="15"/>
     </row>
     <row r="3" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A3" s="5">
+      <c r="A3" s="23">
         <v>2</v>
       </c>
-      <c r="B3" s="9">
+      <c r="B3" s="12">
         <v>43248</v>
       </c>
-      <c r="C3" s="10" t="s">
+      <c r="C3" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D3" s="11" t="s">
+      <c r="D3" s="14" t="s">
         <v>43</v>
       </c>
-      <c r="E3" s="10"/>
-      <c r="F3" s="16" t="s">
+      <c r="E3" s="13"/>
+      <c r="F3" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G3" s="10" t="s">
-        <v>37</v>
-      </c>
-      <c r="H3" s="10" t="s">
+      <c r="G3" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H3" s="13" t="s">
         <v>78</v>
       </c>
     </row>
@@ -1006,28 +993,24 @@
       </c>
     </row>
     <row r="5" spans="1:8" ht="45" x14ac:dyDescent="0.25">
-      <c r="A5" s="5">
+      <c r="A5" s="29">
         <v>4</v>
       </c>
-      <c r="B5" s="24">
+      <c r="B5" s="25">
         <v>43248</v>
       </c>
-      <c r="C5" s="25" t="s">
+      <c r="C5" s="27" t="s">
         <v>12</v>
       </c>
       <c r="D5" s="26" t="s">
         <v>55</v>
       </c>
-      <c r="E5" s="25"/>
-      <c r="F5" s="27" t="s">
-        <v>56</v>
-      </c>
-      <c r="G5" s="25" t="s">
+      <c r="E5" s="27"/>
+      <c r="F5" s="30"/>
+      <c r="G5" s="27" t="s">
         <v>39</v>
       </c>
-      <c r="H5" s="25" t="s">
-        <v>79</v>
-      </c>
+      <c r="H5" s="27"/>
     </row>
     <row r="6" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A6" s="5">
@@ -1125,23 +1108,23 @@
       <c r="A10" s="5">
         <v>9</v>
       </c>
-      <c r="B10" s="28">
+      <c r="B10" s="12">
         <v>43248</v>
       </c>
-      <c r="C10" s="29" t="s">
+      <c r="C10" s="13" t="s">
         <v>12</v>
       </c>
-      <c r="D10" s="30" t="s">
+      <c r="D10" s="14" t="s">
         <v>47</v>
       </c>
-      <c r="E10" s="29"/>
-      <c r="F10" s="31" t="s">
+      <c r="E10" s="13"/>
+      <c r="F10" s="15" t="s">
         <v>56</v>
       </c>
-      <c r="G10" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H10" s="29"/>
+      <c r="G10" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="H10" s="13"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
@@ -1235,23 +1218,23 @@
       <c r="A15" s="5">
         <v>14</v>
       </c>
-      <c r="B15" s="28">
+      <c r="B15" s="9">
         <v>43248</v>
       </c>
-      <c r="C15" s="29" t="s">
+      <c r="C15" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="11" t="s">
         <v>53</v>
       </c>
-      <c r="E15" s="29"/>
-      <c r="F15" s="31" t="s">
+      <c r="E15" s="10"/>
+      <c r="F15" s="16" t="s">
         <v>56</v>
       </c>
-      <c r="G15" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H15" s="29"/>
+      <c r="G15" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H15" s="10"/>
     </row>
     <row r="16" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
@@ -1274,7 +1257,7 @@
         <v>36</v>
       </c>
       <c r="H16" s="13" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
@@ -1291,55 +1274,57 @@
         <v>60</v>
       </c>
       <c r="E17" s="18"/>
-      <c r="F17" s="20" t="s">
-        <v>29</v>
-      </c>
+      <c r="F17" s="20"/>
       <c r="G17" s="18" t="s">
         <v>37</v>
       </c>
       <c r="H17" s="18" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="18" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A18" s="5">
         <v>17</v>
       </c>
-      <c r="B18" s="28">
+      <c r="B18" s="9">
         <v>43256</v>
       </c>
-      <c r="C18" s="29" t="s">
+      <c r="C18" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="30" t="s">
+      <c r="D18" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="E18" s="29"/>
-      <c r="F18" s="29"/>
-      <c r="G18" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H18" s="29"/>
+      <c r="E18" s="10"/>
+      <c r="F18" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G18" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>18</v>
       </c>
-      <c r="B19" s="28">
+      <c r="B19" s="25">
         <v>43256</v>
       </c>
-      <c r="C19" s="30" t="s">
+      <c r="C19" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="30" t="s">
+      <c r="D19" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="E19" s="29"/>
-      <c r="F19" s="29"/>
-      <c r="G19" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H19" s="29"/>
+      <c r="E19" s="27"/>
+      <c r="F19" s="27"/>
+      <c r="G19" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="H19" s="27" t="s">
+        <v>86</v>
+      </c>
     </row>
     <row r="20" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A20" s="5">
@@ -1367,21 +1352,23 @@
       <c r="A21" s="5">
         <v>20</v>
       </c>
-      <c r="B21" s="28">
+      <c r="B21" s="9">
         <v>43256</v>
       </c>
-      <c r="C21" s="29" t="s">
+      <c r="C21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="30" t="s">
+      <c r="D21" s="11" t="s">
         <v>64</v>
       </c>
-      <c r="E21" s="29"/>
-      <c r="F21" s="29"/>
-      <c r="G21" s="29" t="s">
-        <v>39</v>
-      </c>
-      <c r="H21" s="29"/>
+      <c r="E21" s="10"/>
+      <c r="F21" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G21" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A22" s="4">
@@ -1461,8 +1448,12 @@
         <v>68</v>
       </c>
       <c r="E25" s="13"/>
-      <c r="F25" s="13"/>
-      <c r="G25" s="13"/>
+      <c r="F25" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="G25" s="13" t="s">
+        <v>36</v>
+      </c>
       <c r="H25" s="13"/>
     </row>
     <row r="26" spans="1:8" ht="45" x14ac:dyDescent="0.25">
@@ -1486,7 +1477,7 @@
         <v>36</v>
       </c>
       <c r="H26" s="13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="27" spans="1:8" ht="90" x14ac:dyDescent="0.25">
@@ -1515,39 +1506,41 @@
       <c r="A28" s="5">
         <v>27</v>
       </c>
-      <c r="B28" s="32">
+      <c r="B28" s="25">
         <v>43256</v>
       </c>
-      <c r="C28" s="33" t="s">
+      <c r="C28" s="26" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="33" t="s">
+      <c r="D28" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="E28" s="34"/>
-      <c r="F28" s="34"/>
-      <c r="G28" s="34"/>
-      <c r="H28" s="34"/>
+      <c r="E28" s="27"/>
+      <c r="F28" s="27"/>
+      <c r="G28" s="27"/>
+      <c r="H28" s="27"/>
     </row>
     <row r="29" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A29" s="5">
         <v>28</v>
       </c>
-      <c r="B29" s="12">
+      <c r="B29" s="9">
         <v>43257</v>
       </c>
-      <c r="C29" s="13" t="s">
+      <c r="C29" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D29" s="14" t="s">
+      <c r="D29" s="11" t="s">
         <v>72</v>
       </c>
-      <c r="E29" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F29" s="13"/>
-      <c r="G29" s="13"/>
-      <c r="H29" s="13"/>
+      <c r="E29" s="10"/>
+      <c r="F29" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G29" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H29" s="10"/>
     </row>
     <row r="30" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="5">
@@ -1593,98 +1586,120 @@
       <c r="A32" s="4">
         <v>31</v>
       </c>
-      <c r="B32" s="28">
+      <c r="B32" s="25">
         <v>43257</v>
       </c>
-      <c r="C32" s="29" t="s">
+      <c r="C32" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D32" s="30" t="s">
+      <c r="D32" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="E32" s="29" t="s">
+      <c r="E32" s="27" t="s">
         <v>32</v>
       </c>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
+      <c r="F32" s="27"/>
+      <c r="G32" s="27"/>
+      <c r="H32" s="27"/>
     </row>
     <row r="33" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A33" s="5">
         <v>32</v>
       </c>
-      <c r="B33" s="32">
+      <c r="B33" s="25">
         <v>43257</v>
       </c>
-      <c r="C33" s="34" t="s">
+      <c r="C33" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D33" s="33" t="s">
+      <c r="D33" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="E33" s="34"/>
-      <c r="F33" s="34"/>
-      <c r="G33" s="34"/>
-      <c r="H33" s="34"/>
+      <c r="E33" s="27"/>
+      <c r="F33" s="27"/>
+      <c r="G33" s="27"/>
+      <c r="H33" s="27"/>
     </row>
     <row r="34" spans="1:8" ht="30" x14ac:dyDescent="0.25">
-      <c r="A34" s="5">
+      <c r="A34" s="28">
         <v>33</v>
       </c>
-      <c r="B34" s="28">
+      <c r="B34" s="9">
         <v>43257</v>
       </c>
-      <c r="C34" s="29" t="s">
+      <c r="C34" s="10" t="s">
         <v>12</v>
       </c>
-      <c r="D34" s="30" t="s">
+      <c r="D34" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="29"/>
-      <c r="G34" s="29"/>
-      <c r="H34" s="29"/>
+      <c r="E34" s="10"/>
+      <c r="F34" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="G34" s="10" t="s">
+        <v>37</v>
+      </c>
+      <c r="H34" s="10"/>
     </row>
     <row r="35" spans="1:8" ht="90.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A35" s="5">
         <v>34</v>
       </c>
-      <c r="B35" s="35">
+      <c r="B35" s="24">
         <v>43271</v>
       </c>
       <c r="C35" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D35" s="7" t="s">
-        <v>83</v>
+        <v>82</v>
+      </c>
+      <c r="F35" s="6" t="s">
+        <v>29</v>
       </c>
     </row>
     <row r="36" spans="1:8" ht="90" x14ac:dyDescent="0.25">
       <c r="A36" s="5">
         <v>35</v>
       </c>
-      <c r="B36" s="35">
+      <c r="B36" s="24">
         <v>43271</v>
       </c>
       <c r="C36" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D36" s="7" t="s">
-        <v>84</v>
+        <v>83</v>
+      </c>
+      <c r="F36" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G36" s="6" t="s">
+        <v>36</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="120" x14ac:dyDescent="0.25">
       <c r="A37" s="4">
         <v>36</v>
       </c>
-      <c r="B37" s="35">
+      <c r="B37" s="24">
         <v>43271</v>
       </c>
       <c r="C37" s="6" t="s">
         <v>12</v>
       </c>
       <c r="D37" s="7" t="s">
-        <v>85</v>
+        <v>84</v>
+      </c>
+      <c r="F37" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="G37" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H37" s="6" t="s">
+        <v>87</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>